<commit_message>
merged 2 special parameter files
</commit_message>
<xml_diff>
--- a/input/params_special.xlsx
+++ b/input/params_special.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work Projects\cpv\input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="5235" windowWidth="27645" windowHeight="8190" tabRatio="500"/>
   </bookViews>
@@ -197,7 +202,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,6 +385,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -427,7 +435,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -462,7 +470,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -673,9 +681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,6 +774,15 @@
       <c r="J2" s="10" t="s">
         <v>50</v>
       </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>999</v>
+      </c>
+      <c r="M2">
+        <v>999</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -798,6 +815,15 @@
       <c r="J3" s="10" t="s">
         <v>50</v>
       </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>999</v>
+      </c>
+      <c r="M3">
+        <v>999</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -830,6 +856,15 @@
       <c r="J4" s="10" t="s">
         <v>50</v>
       </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>999</v>
+      </c>
+      <c r="M4">
+        <v>999</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -865,6 +900,12 @@
       <c r="K5">
         <v>2</v>
       </c>
+      <c r="L5">
+        <v>999</v>
+      </c>
+      <c r="M5">
+        <v>999</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -900,6 +941,12 @@
       <c r="K6">
         <v>2</v>
       </c>
+      <c r="L6">
+        <v>999</v>
+      </c>
+      <c r="M6">
+        <v>999</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -935,6 +982,12 @@
       <c r="K7">
         <v>2</v>
       </c>
+      <c r="L7">
+        <v>999</v>
+      </c>
+      <c r="M7">
+        <v>999</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -970,6 +1023,12 @@
       <c r="K8">
         <v>2</v>
       </c>
+      <c r="L8">
+        <v>999</v>
+      </c>
+      <c r="M8">
+        <v>999</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -1005,6 +1064,12 @@
       <c r="K9">
         <v>2</v>
       </c>
+      <c r="L9">
+        <v>999</v>
+      </c>
+      <c r="M9">
+        <v>999</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -1040,6 +1105,12 @@
       <c r="K10">
         <v>2</v>
       </c>
+      <c r="L10">
+        <v>999</v>
+      </c>
+      <c r="M10">
+        <v>999</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -1075,6 +1146,12 @@
       <c r="K11">
         <v>2</v>
       </c>
+      <c r="L11">
+        <v>999</v>
+      </c>
+      <c r="M11">
+        <v>999</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -1110,6 +1187,12 @@
       <c r="K12">
         <v>2</v>
       </c>
+      <c r="L12">
+        <v>999</v>
+      </c>
+      <c r="M12">
+        <v>999</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -1145,6 +1228,12 @@
       <c r="K13">
         <v>2</v>
       </c>
+      <c r="L13">
+        <v>999</v>
+      </c>
+      <c r="M13">
+        <v>999</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -1180,6 +1269,12 @@
       <c r="K14">
         <v>2</v>
       </c>
+      <c r="L14">
+        <v>999</v>
+      </c>
+      <c r="M14">
+        <v>999</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -1215,6 +1310,12 @@
       <c r="K15" s="11" t="s">
         <v>53</v>
       </c>
+      <c r="L15">
+        <v>999</v>
+      </c>
+      <c r="M15">
+        <v>999</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -1250,8 +1351,14 @@
       <c r="K16" s="11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>999</v>
+      </c>
+      <c r="M16">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
@@ -1285,8 +1392,14 @@
       <c r="K17" s="11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>999</v>
+      </c>
+      <c r="M17">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
@@ -1320,8 +1433,14 @@
       <c r="K18" s="11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>999</v>
+      </c>
+      <c r="M18">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
@@ -1355,8 +1474,14 @@
       <c r="K19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>999</v>
+      </c>
+      <c r="M19">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -1390,8 +1515,14 @@
       <c r="K20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>999</v>
+      </c>
+      <c r="M20">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1425,8 +1556,14 @@
       <c r="K21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>999</v>
+      </c>
+      <c r="M21">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>18</v>
       </c>
@@ -1460,8 +1597,14 @@
       <c r="K22" s="11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>999</v>
+      </c>
+      <c r="M22">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>18</v>
       </c>
@@ -1495,8 +1638,14 @@
       <c r="K23" s="11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>999</v>
+      </c>
+      <c r="M23">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>18</v>
       </c>
@@ -1530,8 +1679,14 @@
       <c r="K24" s="11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>999</v>
+      </c>
+      <c r="M24">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>18</v>
       </c>
@@ -1564,6 +1719,12 @@
       </c>
       <c r="K25" s="11" t="s">
         <v>53</v>
+      </c>
+      <c r="L25">
+        <v>999</v>
+      </c>
+      <c r="M25">
+        <v>999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue incorrectly selecting the highest indx
</commit_message>
<xml_diff>
--- a/input/params_special.xlsx
+++ b/input/params_special.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$27</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="62">
   <si>
     <t>emi_master</t>
   </si>
@@ -200,6 +200,21 @@
   </si>
   <si>
     <t>COMP_MIN_THICKNESS</t>
+  </si>
+  <si>
+    <t>COAT_MIN_THICKNESS</t>
+  </si>
+  <si>
+    <t>COAT_MAX_THICKNESS</t>
+  </si>
+  <si>
+    <t>PP_CM_IPT_W</t>
+  </si>
+  <si>
+    <t>COMP_MEAN_WEIGHT</t>
+  </si>
+  <si>
+    <t>COAT_MEAN_WEIGHT</t>
   </si>
 </sst>
 </file>
@@ -670,7 +685,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1402,16 +1417,16 @@
         <v>8</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G18" s="6">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>10</v>
@@ -1420,7 +1435,7 @@
         <v>16</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K18" s="4">
         <v>2</v>
@@ -1433,26 +1448,26 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>12</v>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="G19" s="6">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>10</v>
@@ -1460,11 +1475,11 @@
       <c r="I19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K19" s="4">
-        <v>2</v>
+      <c r="J19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="L19" s="4">
         <v>999</v>
@@ -1484,16 +1499,16 @@
         <v>26</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G20" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>10</v>
@@ -1525,16 +1540,16 @@
         <v>26</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="G21" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>10</v>
@@ -1542,8 +1557,8 @@
       <c r="I21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J21" s="4" t="s">
-        <v>38</v>
+      <c r="J21" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>40</v>
@@ -1566,16 +1581,16 @@
         <v>26</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="G22" s="6">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>10</v>
@@ -1597,26 +1612,26 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>49</v>
+      <c r="C23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G23" s="6">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>10</v>
@@ -1625,20 +1640,188 @@
         <v>16</v>
       </c>
       <c r="J23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" s="4">
+        <v>2</v>
+      </c>
+      <c r="L23" s="4">
+        <v>999</v>
+      </c>
+      <c r="M23" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="6">
+        <v>3</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K23" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L23" s="4">
-        <v>999</v>
-      </c>
-      <c r="M23" s="4">
+      <c r="K24" s="4">
+        <v>2</v>
+      </c>
+      <c r="L24" s="4">
+        <v>999</v>
+      </c>
+      <c r="M24" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="6">
+        <v>5</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K25" s="4">
+        <v>2</v>
+      </c>
+      <c r="L25" s="4">
+        <v>999</v>
+      </c>
+      <c r="M25" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="6">
+        <v>8</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" s="4">
+        <v>2</v>
+      </c>
+      <c r="L26" s="4">
+        <v>999</v>
+      </c>
+      <c r="M26" s="4">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="6">
+        <v>10</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" s="4">
+        <v>2</v>
+      </c>
+      <c r="L27" s="4">
+        <v>999</v>
+      </c>
+      <c r="M27" s="4">
         <v>999</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M23"/>
+  <autoFilter ref="A1:M27">
+    <sortState ref="A2:M23">
+      <sortCondition ref="G1:G23"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:N223">
     <sortCondition ref="A2:A223"/>
     <sortCondition ref="B2:B223"/>

</xml_diff>

<commit_message>
working on spec extraction
</commit_message>
<xml_diff>
--- a/input/params_special.xlsx
+++ b/input/params_special.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="60">
   <si>
     <t>emi_master</t>
   </si>
@@ -152,12 +152,6 @@
   </si>
   <si>
     <t>ss</t>
-  </si>
-  <si>
-    <t>range_min</t>
-  </si>
-  <si>
-    <t>range_max</t>
   </si>
   <si>
     <t>EMI_0701</t>
@@ -685,11 +679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,12 +698,10 @@
     <col min="8" max="9" width="15.28515625" style="7" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" style="4" customWidth="1"/>
     <col min="11" max="11" width="19" style="4" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="4" customWidth="1"/>
-    <col min="14" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="12" max="1023" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -723,7 +715,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>25</v>
@@ -743,14 +735,8 @@
       <c r="K1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
@@ -784,14 +770,8 @@
       <c r="K2" s="4">
         <v>2</v>
       </c>
-      <c r="L2" s="4">
-        <v>999</v>
-      </c>
-      <c r="M2" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
@@ -808,7 +788,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G3" s="6">
         <v>2</v>
@@ -825,14 +805,8 @@
       <c r="K3" s="4">
         <v>2</v>
       </c>
-      <c r="L3" s="4">
-        <v>999</v>
-      </c>
-      <c r="M3" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -849,7 +823,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G4" s="6">
         <v>4</v>
@@ -866,14 +840,8 @@
       <c r="K4" s="4">
         <v>2</v>
       </c>
-      <c r="L4" s="4">
-        <v>999</v>
-      </c>
-      <c r="M4" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>20</v>
       </c>
@@ -907,14 +875,8 @@
       <c r="K5" s="4">
         <v>2</v>
       </c>
-      <c r="L5" s="4">
-        <v>999</v>
-      </c>
-      <c r="M5" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>20</v>
       </c>
@@ -931,7 +893,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G6" s="6">
         <v>7</v>
@@ -948,14 +910,8 @@
       <c r="K6" s="4">
         <v>2</v>
       </c>
-      <c r="L6" s="4">
-        <v>999</v>
-      </c>
-      <c r="M6" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
@@ -972,7 +928,7 @@
         <v>18</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G7" s="6">
         <v>9</v>
@@ -989,19 +945,13 @@
       <c r="K7" s="4">
         <v>2</v>
       </c>
-      <c r="L7" s="4">
-        <v>999</v>
-      </c>
-      <c r="M7" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>8</v>
@@ -1013,7 +963,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G8" s="6">
         <v>11</v>
@@ -1022,7 +972,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>38</v>
@@ -1030,19 +980,13 @@
       <c r="K8" s="4">
         <v>2</v>
       </c>
-      <c r="L8" s="4">
-        <v>999</v>
-      </c>
-      <c r="M8" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>8</v>
@@ -1054,7 +998,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G9" s="6">
         <v>13</v>
@@ -1063,7 +1007,7 @@
         <v>10</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>39</v>
@@ -1071,19 +1015,13 @@
       <c r="K9" s="4">
         <v>2</v>
       </c>
-      <c r="L9" s="4">
-        <v>999</v>
-      </c>
-      <c r="M9" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>8</v>
@@ -1095,7 +1033,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G10" s="6">
         <v>15</v>
@@ -1104,7 +1042,7 @@
         <v>10</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>38</v>
@@ -1112,19 +1050,13 @@
       <c r="K10" s="4">
         <v>2</v>
       </c>
-      <c r="L10" s="4">
-        <v>999</v>
-      </c>
-      <c r="M10" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>8</v>
@@ -1136,7 +1068,7 @@
         <v>18</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G11" s="6">
         <v>17</v>
@@ -1145,7 +1077,7 @@
         <v>10</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>39</v>
@@ -1153,14 +1085,8 @@
       <c r="K11" s="4">
         <v>2</v>
       </c>
-      <c r="L11" s="4">
-        <v>999</v>
-      </c>
-      <c r="M11" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>14</v>
       </c>
@@ -1194,14 +1120,8 @@
       <c r="K12" s="4">
         <v>2</v>
       </c>
-      <c r="L12" s="4">
-        <v>999</v>
-      </c>
-      <c r="M12" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>14</v>
       </c>
@@ -1235,14 +1155,8 @@
       <c r="K13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L13" s="4">
-        <v>999</v>
-      </c>
-      <c r="M13" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>14</v>
       </c>
@@ -1253,13 +1167,13 @@
         <v>26</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G14" s="6">
         <v>21</v>
@@ -1276,14 +1190,8 @@
       <c r="K14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L14" s="4">
-        <v>999</v>
-      </c>
-      <c r="M14" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>14</v>
       </c>
@@ -1317,14 +1225,8 @@
       <c r="K15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="4">
-        <v>999</v>
-      </c>
-      <c r="M15" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1335,13 +1237,13 @@
         <v>26</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G16" s="6">
         <v>23</v>
@@ -1358,14 +1260,8 @@
       <c r="K16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L16" s="4">
-        <v>999</v>
-      </c>
-      <c r="M16" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
@@ -1399,14 +1295,8 @@
       <c r="K17" s="4">
         <v>2</v>
       </c>
-      <c r="L17" s="4">
-        <v>999</v>
-      </c>
-      <c r="M17" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>14</v>
       </c>
@@ -1423,7 +1313,7 @@
         <v>18</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G18" s="6">
         <v>26</v>
@@ -1440,14 +1330,8 @@
       <c r="K18" s="4">
         <v>2</v>
       </c>
-      <c r="L18" s="4">
-        <v>999</v>
-      </c>
-      <c r="M18" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>14</v>
       </c>
@@ -1481,14 +1365,8 @@
       <c r="K19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L19" s="4">
-        <v>999</v>
-      </c>
-      <c r="M19" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>14</v>
       </c>
@@ -1499,13 +1377,13 @@
         <v>26</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G20" s="6">
         <v>29</v>
@@ -1522,14 +1400,8 @@
       <c r="K20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L20" s="4">
-        <v>999</v>
-      </c>
-      <c r="M20" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>14</v>
       </c>
@@ -1563,14 +1435,8 @@
       <c r="K21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L21" s="4">
-        <v>999</v>
-      </c>
-      <c r="M21" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>14</v>
       </c>
@@ -1581,13 +1447,13 @@
         <v>26</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>28</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G22" s="6">
         <v>31</v>
@@ -1604,14 +1470,8 @@
       <c r="K22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L22" s="4">
-        <v>999</v>
-      </c>
-      <c r="M22" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>14</v>
       </c>
@@ -1628,7 +1488,7 @@
         <v>18</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G23" s="6">
         <v>32</v>
@@ -1645,14 +1505,8 @@
       <c r="K23" s="4">
         <v>2</v>
       </c>
-      <c r="L23" s="4">
-        <v>999</v>
-      </c>
-      <c r="M23" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>14</v>
       </c>
@@ -1669,7 +1523,7 @@
         <v>18</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G24" s="6">
         <v>3</v>
@@ -1686,14 +1540,8 @@
       <c r="K24" s="4">
         <v>2</v>
       </c>
-      <c r="L24" s="4">
-        <v>999</v>
-      </c>
-      <c r="M24" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>14</v>
       </c>
@@ -1710,7 +1558,7 @@
         <v>18</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G25" s="6">
         <v>5</v>
@@ -1727,14 +1575,8 @@
       <c r="K25" s="4">
         <v>2</v>
       </c>
-      <c r="L25" s="4">
-        <v>999</v>
-      </c>
-      <c r="M25" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>14</v>
       </c>
@@ -1745,13 +1587,13 @@
         <v>8</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G26" s="6">
         <v>8</v>
@@ -1768,14 +1610,8 @@
       <c r="K26" s="4">
         <v>2</v>
       </c>
-      <c r="L26" s="4">
-        <v>999</v>
-      </c>
-      <c r="M26" s="4">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>14</v>
       </c>
@@ -1786,13 +1622,13 @@
         <v>8</v>
       </c>
       <c r="D27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="G27" s="6">
         <v>10</v>
@@ -1809,15 +1645,9 @@
       <c r="K27" s="4">
         <v>2</v>
       </c>
-      <c r="L27" s="4">
-        <v>999</v>
-      </c>
-      <c r="M27" s="4">
-        <v>999</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M27">
+  <autoFilter ref="A1:K27">
     <sortState ref="A2:M23">
       <sortCondition ref="G1:G23"/>
     </sortState>

</xml_diff>

<commit_message>
Renamed COMP_MEAN_WEIGHT to COMP_WEIGHT_MEAN
</commit_message>
<xml_diff>
--- a/input/params_special.xlsx
+++ b/input/params_special.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sobczakk\OneDrive - Takeda\Documents\GIT REPOS\cpv\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="11_34C2B377663F4BAD935724B84C902A23CE857F24" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{5D8ADB74-CCB8-4C05-8623-A5A072A5A83B}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="102_{D9E7DF95-67E1-4BF1-84CE-C352D2159D46}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{8AB1D8F7-A023-491C-9F45-287ACB9B908C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="3120" windowWidth="21315" windowHeight="12165" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -206,9 +206,6 @@
     <t>PP_CM_IPT_W</t>
   </si>
   <si>
-    <t>COMP_MEAN_WEIGHT</t>
-  </si>
-  <si>
     <t>COAT_MEAN_WEIGHT</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
     <t>Weight/Thickness/Hardness IPTs: 50%</t>
   </si>
   <si>
-    <t>COMP_MEAN_WEIGHT_MIDDLE</t>
-  </si>
-  <si>
     <t>COMP_MAX_THICKNESS_MIDDLE</t>
   </si>
   <si>
@@ -230,46 +224,52 @@
     <t>PP_CM_IPT_W_%CV</t>
   </si>
   <si>
-    <t>COMP_MEAN_WEIGHT_CV_MIDDLE</t>
-  </si>
-  <si>
     <t>COMP_AVG_HARDNESS_MIDDLE</t>
   </si>
   <si>
     <t>Weight/Thickness/Hardness IPTs: 90%</t>
   </si>
   <si>
-    <t>COMP_MEAN_WEIGHT_END</t>
-  </si>
-  <si>
     <t>COMP_MAX_THICKNESS_END</t>
   </si>
   <si>
     <t>COMP_MIN_THICKNESS_END</t>
   </si>
   <si>
-    <t>COMP_MEAN_WEIGHT_CV_END</t>
-  </si>
-  <si>
     <t>COMP_AVG_HARDNESS_END</t>
   </si>
   <si>
     <t>Weight/Thickness/Hardness IPTs:1st TIC</t>
   </si>
   <si>
-    <t>COMP_MEAN_WEIGHT_START</t>
-  </si>
-  <si>
     <t>COMP_MAX_THICKNESS_START</t>
   </si>
   <si>
     <t>COMP_MIN_THICKNESS_START</t>
   </si>
   <si>
-    <t>COMP_MEAN_WEIGHT_CV_START</t>
-  </si>
-  <si>
     <t>COMP_AVG_HARDNESS_START</t>
+  </si>
+  <si>
+    <t>COMP_WEIGHT_MEAN</t>
+  </si>
+  <si>
+    <t>COMP_WEIGHT_MEAN_MIDDLE</t>
+  </si>
+  <si>
+    <t>COMP_WEIGHT_MEAN_CV_MIDDLE</t>
+  </si>
+  <si>
+    <t>COMP_WEIGHT_MEAN_END</t>
+  </si>
+  <si>
+    <t>COMP_WEIGHT_MEAN_CV_END</t>
+  </si>
+  <si>
+    <t>COMP_WEIGHT_MEAN_START</t>
+  </si>
+  <si>
+    <t>COMP_WEIGHT_MEAN_CV_START</t>
   </si>
 </sst>
 </file>
@@ -778,7 +778,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G58" sqref="G58"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +985,7 @@
         <v>47</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>51</v>
@@ -1020,7 +1020,7 @@
         <v>27</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>33</v>
@@ -1055,7 +1055,7 @@
         <v>46</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>50</v>
@@ -1090,7 +1090,7 @@
         <v>29</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>31</v>
@@ -1125,7 +1125,7 @@
         <v>47</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>51</v>
@@ -1160,7 +1160,7 @@
         <v>27</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>33</v>
@@ -1195,7 +1195,7 @@
         <v>46</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>50</v>
@@ -1230,7 +1230,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>31</v>
@@ -1968,7 +1968,7 @@
         <v>18</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G34" s="6">
         <v>10</v>
@@ -2038,7 +2038,7 @@
         <v>18</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="G36" s="6">
         <v>8</v>
@@ -2315,10 +2315,10 @@
         <v>57</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="G44" s="6">
         <v>49</v>
@@ -2350,10 +2350,10 @@
         <v>13</v>
       </c>
       <c r="E45" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>63</v>
       </c>
       <c r="G45" s="6">
         <v>50</v>
@@ -2385,10 +2385,10 @@
         <v>12</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G46" s="6">
         <v>51</v>
@@ -2417,13 +2417,13 @@
         <v>8</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G47" s="6">
         <v>52</v>
@@ -2455,10 +2455,10 @@
         <v>9</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G48" s="6">
         <v>53</v>
@@ -2490,10 +2490,10 @@
         <v>57</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G49" s="6">
         <v>54</v>
@@ -2525,10 +2525,10 @@
         <v>13</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G50" s="6">
         <v>55</v>
@@ -2560,10 +2560,10 @@
         <v>12</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G51" s="6">
         <v>56</v>
@@ -2592,13 +2592,13 @@
         <v>8</v>
       </c>
       <c r="D52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E52" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="F52" s="12" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G52" s="6">
         <v>57</v>
@@ -2630,10 +2630,10 @@
         <v>9</v>
       </c>
       <c r="E53" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F53" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="G53" s="6">
         <v>58</v>
@@ -2665,10 +2665,10 @@
         <v>57</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G54" s="6">
         <v>59</v>
@@ -2700,10 +2700,10 @@
         <v>13</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G55" s="6">
         <v>60</v>
@@ -2735,10 +2735,10 @@
         <v>12</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G56" s="6">
         <v>61</v>
@@ -2767,13 +2767,13 @@
         <v>8</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G57" s="6">
         <v>62</v>
@@ -2805,10 +2805,10 @@
         <v>9</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G58" s="6">
         <v>63</v>

</xml_diff>